<commit_message>
CGP baseline max back init
</commit_message>
<xml_diff>
--- a/RV-results.xlsx
+++ b/RV-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarinov-notas\dev\cgp-optimization-experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{06A586A8-C204-49FD-AF89-5C237B258D06}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CEBF349A-B8EC-4EBA-9E87-D3BD2DAD7D26}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6750" activeTab="1" xr2:uid="{EDB30DD8-1982-4DCD-87F2-B5E5C07C38C6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Nguyen 4</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>PSO, gen=200, pop=50, default params, max_back=10</t>
+  </si>
+  <si>
+    <t>Pagie 1</t>
+  </si>
+  <si>
+    <t>Keijzer 6</t>
+  </si>
+  <si>
+    <t>Vladislasleva 4</t>
+  </si>
+  <si>
+    <t>PSO, gen=200, pop=50, default params, max_back=10, FIPS, von nouman</t>
+  </si>
+  <si>
+    <t>CGP single mutation, 50, ptree data</t>
+  </si>
+  <si>
+    <t>3h30min</t>
   </si>
 </sst>
 </file>
@@ -218,7 +236,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -231,6 +249,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40 % - zvýraznenie3" xfId="3" builtinId="39"/>
@@ -881,22 +901,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BD5ECB-2399-4152-B4E0-4FED036DED18}">
-  <dimension ref="A2:X14"/>
+  <dimension ref="A2:AT16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="1.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="1.7109375" style="7" customWidth="1"/>
     <col min="12" max="12" width="1.7109375" style="7" customWidth="1"/>
     <col min="17" max="17" width="1.7109375" style="7" customWidth="1"/>
+    <col min="22" max="22" width="1.7109375" style="7" customWidth="1"/>
+    <col min="27" max="27" width="1.7109375" style="7" customWidth="1"/>
+    <col min="32" max="32" width="1.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -924,8 +947,29 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
-    </row>
-    <row r="3" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V2" s="12"/>
+      <c r="W2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+    </row>
+    <row r="3" spans="1:46" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
@@ -977,8 +1021,47 @@
       <c r="U3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="13"/>
+      <c r="W3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1030,372 +1113,449 @@
       <c r="U4">
         <v>8.0979999999999996E-2</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AK4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
+      <c r="H5" s="2">
+        <v>5.8E-20</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.9910000000000001E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.6E-2</v>
+      </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="R5">
+        <v>1.095</v>
+      </c>
+      <c r="S5">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="T5">
+        <v>1.0976999999999999</v>
+      </c>
+      <c r="U5" s="2">
+        <v>6.0100000000000001E-6</v>
+      </c>
+      <c r="W5">
+        <v>4.5690000000000001E-3</v>
+      </c>
+      <c r="X5">
+        <v>0.20396</v>
+      </c>
+      <c r="Y5">
+        <v>0.20036000000000001</v>
+      </c>
+      <c r="Z5">
+        <v>1.163E-2</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>2.2200000000000001E-5</v>
+      </c>
+      <c r="AC5">
+        <v>3.8719999999999997E-2</v>
+      </c>
+      <c r="AD5">
+        <v>8.0499999999999999E-3</v>
+      </c>
+      <c r="AE5">
+        <v>1.2787E-2</v>
+      </c>
+      <c r="AG5">
+        <v>2.12E-2</v>
+      </c>
+      <c r="AH5">
+        <v>3.3874899999999999E-2</v>
+      </c>
+      <c r="AI5">
+        <v>3.4049999999999997E-2</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>1.696E-5</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="AK7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO7" s="7"/>
+      <c r="AT7" s="7"/>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.3</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>0.24</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>3.0099999999999998E-2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H8" s="1">
         <v>1.6100000000000001E-4</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I8" s="1">
         <v>1.07E-3</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J8" s="1">
         <v>1.1199999999999999E-3</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K8" s="2">
         <v>6.7900000000000006E-8</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M8" s="1">
         <v>1.0869999999999999E-2</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N8" s="1">
         <v>3.4599999999999999E-2</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O8" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P8" s="2">
         <v>7.0240000000000005E-5</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R8" s="1">
         <v>1.16449</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S8" s="1">
         <v>1.76</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T8" s="1">
         <v>1.4119999999999999</v>
       </c>
-      <c r="U7" s="1">
+      <c r="U8" s="1">
         <v>0.19769999999999999</v>
       </c>
-      <c r="W7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="AK8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO8" s="7"/>
+      <c r="AT8" s="7"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1.67E-3</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>3.27E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>1.95E-2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F9" s="1">
         <v>1.5E-3</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <v>2.3099999999999999E-6</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I9" s="1">
         <v>2.7599999999999999E-4</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J9" s="1">
         <v>1.8929999999999999E-4</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K9" s="2">
         <v>6.0119999999999998E-8</v>
       </c>
-      <c r="M8">
+      <c r="M9">
         <v>4.0190000000000001E-4</v>
       </c>
-      <c r="N8">
+      <c r="N9">
         <v>6.9800000000000001E-3</v>
       </c>
-      <c r="O8">
+      <c r="O9">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P9" s="2">
         <v>2.73E-5</v>
       </c>
-      <c r="R8">
+      <c r="R9">
         <v>0.64</v>
       </c>
-      <c r="S8">
+      <c r="S9">
         <v>1.2829999999999999</v>
       </c>
-      <c r="T8">
+      <c r="T9">
         <v>1.4159999999999999</v>
       </c>
-      <c r="U8">
+      <c r="U9">
         <v>3.9E-2</v>
       </c>
-      <c r="W8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="AK9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO9" s="7"/>
+      <c r="AT9" s="7"/>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2.8E-3</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>0.107</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>1.9199999999999999E-5</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I10" s="1">
         <v>7.6999999999999996E-4</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J10" s="1">
         <v>3.3599999999999998E-4</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K10" s="2">
         <v>1.3900000000000001E-5</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>1.1900000000000001E-3</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>7.26E-3</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P10" s="2">
         <v>8.0970000000000006E-6</v>
       </c>
-      <c r="R9">
+      <c r="R10">
         <v>8.2400000000000001E-2</v>
       </c>
-      <c r="S9">
+      <c r="S10">
         <v>1.32</v>
       </c>
-      <c r="T9">
+      <c r="T10">
         <v>1.42</v>
       </c>
-      <c r="U9">
+      <c r="U10">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="W9" t="s">
-        <v>26</v>
-      </c>
-      <c r="X9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="AK10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO10" s="7"/>
+      <c r="AT10" s="7"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>1.8600000000000001E-3</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>1.8979999999999999</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>2.0979999999999999</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>0.85</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H11" s="11">
         <v>9.7699999999999996E-6</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I11" s="1">
         <v>0.40400000000000003</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J11" s="1">
         <v>0.19370000000000001</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K11" s="1">
         <v>0.13800000000000001</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M11" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N11" s="1">
         <v>0.45</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O11" s="1">
         <v>5.6300000000000003E-2</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P11" s="1">
         <v>0.56298000000000004</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R11" s="1">
         <v>0.27900000000000003</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S11" s="1">
         <v>2.1880000000000002</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T11" s="1">
         <v>2.3199999999999998</v>
       </c>
-      <c r="U10" s="1">
+      <c r="U11" s="1">
         <v>0.16</v>
       </c>
-      <c r="W10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="AK11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO11" s="7"/>
+      <c r="AT11" s="7"/>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>1.04E-2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>0.11700000000000001</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>6.9800000000000001E-2</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>2.5499999999999998E-2</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11">
+      <c r="G12" s="10"/>
+      <c r="H12" s="11">
         <v>7.8100000000000001E-5</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I12" s="1">
         <v>7.7799999999999996E-3</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J12" s="1">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K12" s="2">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M12" s="1">
         <v>3.5599999999999998E-4</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N12" s="1">
         <v>1.04E-2</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O12" s="1">
         <v>9.0900000000000009E-3</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P12" s="11">
         <v>7.5699999999999997E-5</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R12" s="1">
         <v>0.67579599999999995</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S12" s="1">
         <v>1.32</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T12" s="1">
         <v>1.42</v>
       </c>
-      <c r="U11" s="1">
+      <c r="U12" s="1">
         <v>4.0300000000000002E-2</v>
       </c>
-      <c r="W11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>9.7300000000000008E-3</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>0.27179999999999999</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>5.5370000000000003E-2</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <v>3.93E-5</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I13" s="1">
         <v>8.8000000000000003E-4</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J13" s="1">
         <v>8.5999999999999998E-4</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K13" s="2">
         <v>1.5900000000000001E-7</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M13" s="1">
         <v>1.01E-2</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N13" s="1">
         <v>4.19E-2</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O13" s="1">
         <v>3.8899999999999997E-2</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P13" s="11">
         <v>1.34E-4</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R13" s="1">
         <v>1.1126</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S13" s="1">
         <v>2.1480000000000001</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T13" s="1">
         <v>2.3210000000000002</v>
       </c>
-      <c r="U12" s="1">
+      <c r="U13" s="1">
         <v>1.38E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>